<commit_message>
Updated dashboard with new Order Details screen
</commit_message>
<xml_diff>
--- a/data/order_db_v2.xlsx
+++ b/data/order_db_v2.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:AB51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +533,51 @@
           <t>Seller TIN</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Structure</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Thickness</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Width</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Ref</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Carrier</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>AWB</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Tracking Link</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Shipment Status</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Credit Days</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -536,14 +585,12 @@
           <t>ORD-10000</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-08-22</t>
-        </is>
+      <c r="B2" s="2" t="n">
+        <v>45891</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Film Extrusion</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -568,16 +615,14 @@
       <c r="I2" t="n">
         <v>593392.8</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2025-08-26 16:15</t>
-        </is>
+      <c r="J2" s="2" t="n">
+        <v>45952</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -609,6 +654,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>44µ</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>1061mm</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>CUST-KMH3S3</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB2" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="3">
@@ -617,14 +701,12 @@
           <t>ORD-10001</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-06-09</t>
-        </is>
+      <c r="B3" s="2" t="n">
+        <v>45817</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>Printing</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -649,16 +731,14 @@
       <c r="I3" t="n">
         <v>3055360</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2025-06-24 16:15</t>
-        </is>
+      <c r="J3" s="2" t="n">
+        <v>45878</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2025-08-08</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -690,6 +770,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>97µ</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>1046mm</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>CUST-710EMU</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB3" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -698,10 +817,8 @@
           <t>ORD-10002</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-07-23</t>
-        </is>
+      <c r="B4" s="2" t="n">
+        <v>45861</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -730,24 +847,20 @@
       <c r="I4" t="n">
         <v>221734.5</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>2025-07-29 16:15</t>
-        </is>
+      <c r="J4" s="2" t="n">
+        <v>45867.67708333334</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>2025-07-26 16:15</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>2025-07-31 16:15</t>
-        </is>
+      <c r="L4" s="2" t="n">
+        <v>45869.67708333334</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2025-09-21</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -779,6 +892,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>67µ</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>433mm</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>CUST-B51TN5</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Blue Dart</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>316453614319</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>https://example.com/track/316453614319</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -787,10 +943,8 @@
           <t>ORD-10003</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-09-23</t>
-        </is>
+      <c r="B5" s="2" t="n">
+        <v>45923</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -819,24 +973,20 @@
       <c r="I5" t="n">
         <v>4311722.9</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2025-09-28 16:15</t>
-        </is>
+      <c r="J5" s="2" t="n">
+        <v>45928.67708333334</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>2025-09-25 16:15</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>2025-09-27 16:15</t>
-        </is>
+      <c r="L5" s="2" t="n">
+        <v>45927.67708333334</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -868,6 +1018,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>100µ</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>680mm</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>CUST-PQHUMR</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Delhivery</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>614572711320</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>https://example.com/track/614572711320</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB5" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -876,14 +1069,12 @@
           <t>ORD-10004</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-05-29</t>
-        </is>
+      <c r="B6" s="2" t="n">
+        <v>45806</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -908,10 +1099,8 @@
       <c r="I6" t="n">
         <v>2172258</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2025-06-04 16:15</t>
-        </is>
+      <c r="J6" s="2" t="n">
+        <v>45867</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -921,7 +1110,7 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2025-07-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -953,6 +1142,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>104µ</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>979mm</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>CUST-TC4YVW</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>DTDC</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>837063050823</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>https://example.com/track/837063050823</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>In Transit</t>
+        </is>
+      </c>
+      <c r="AB6" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="7">
@@ -961,14 +1193,12 @@
           <t>ORD-10005</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2025-11-13</t>
-        </is>
+      <c r="B7" s="2" t="n">
+        <v>45974</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>Printing</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -993,16 +1223,14 @@
       <c r="I7" t="n">
         <v>2342839.2</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>2025-11-27 16:15</t>
-        </is>
+      <c r="J7" s="2" t="n">
+        <v>46035</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-03-14</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1034,6 +1262,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>82µ</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>1075mm</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>CUST-17Z9IG</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -1042,14 +1309,12 @@
           <t>ORD-10006</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2025-07-04</t>
-        </is>
+      <c r="B8" s="2" t="n">
+        <v>45842</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>QC</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1074,16 +1339,14 @@
       <c r="I8" t="n">
         <v>1012552.4</v>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>2025-07-09 16:15</t>
-        </is>
+      <c r="J8" s="2" t="n">
+        <v>45904</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1115,6 +1378,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>96µ</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>976mm</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>CUST-FNHSZO</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB8" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="9">
@@ -1123,10 +1425,8 @@
           <t>ORD-10007</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2025-09-30</t>
-        </is>
+      <c r="B9" s="2" t="n">
+        <v>45930</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1155,24 +1455,20 @@
       <c r="I9" t="n">
         <v>462346</v>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>2025-10-02 16:15</t>
-        </is>
+      <c r="J9" s="2" t="n">
+        <v>45932.67708333334</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>2025-10-03 16:15</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>2025-10-07 16:15</t>
-        </is>
+      <c r="L9" s="2" t="n">
+        <v>45937.67708333334</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1204,6 +1500,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>115µ</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>966mm</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>CUST-X0SE4F</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>685340604033</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>https://example.com/track/685340604033</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB9" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="10">
@@ -1212,14 +1551,12 @@
           <t>ORD-10008</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2025-06-05</t>
-        </is>
+      <c r="B10" s="2" t="n">
+        <v>45813</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1244,10 +1581,8 @@
       <c r="I10" t="n">
         <v>970515</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>2025-06-08 16:15</t>
-        </is>
+      <c r="J10" s="2" t="n">
+        <v>45874</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1257,7 +1592,7 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2025-08-04</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1289,6 +1624,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>65µ</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>976mm</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>CUST-MZSYDS</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>621201104384</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>https://example.com/track/621201104384</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>In Transit</t>
+        </is>
+      </c>
+      <c r="AB10" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -1297,14 +1675,12 @@
           <t>ORD-10009</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2025-07-29</t>
-        </is>
+      <c r="B11" s="2" t="n">
+        <v>45867</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Printing</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1329,16 +1705,14 @@
       <c r="I11" t="n">
         <v>724530.4</v>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>2025-08-07 16:15</t>
-        </is>
+      <c r="J11" s="2" t="n">
+        <v>45929</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1370,6 +1744,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>85µ</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>444mm</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>CUST-2YCC6A</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB11" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -1378,14 +1791,12 @@
           <t>ORD-10010</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2025-06-21</t>
-        </is>
+      <c r="B12" s="2" t="n">
+        <v>45829</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>Film Extrusion</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1410,16 +1821,14 @@
       <c r="I12" t="n">
         <v>794817.4</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>2025-07-03 16:15</t>
-        </is>
+      <c r="J12" s="2" t="n">
+        <v>45890</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2025-08-20</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1451,6 +1860,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>101µ</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>643mm</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>CUST-OD5J2J</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB12" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -1459,10 +1907,8 @@
           <t>ORD-10011</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2025-07-02</t>
-        </is>
+      <c r="B13" s="2" t="n">
+        <v>45840</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1491,24 +1937,20 @@
       <c r="I13" t="n">
         <v>1489030</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>2025-07-04 16:15</t>
-        </is>
+      <c r="J13" s="2" t="n">
+        <v>45842.67708333334</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>2025-07-03 16:15</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>2025-07-08 16:15</t>
-        </is>
+      <c r="L13" s="2" t="n">
+        <v>45846.67708333334</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2025-08-31</t>
+          <t>2025-09-06</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1540,6 +1982,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>81µ</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>524mm</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>CUST-6TB815</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>175564454120</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>https://example.com/track/175564454120</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB13" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -1548,10 +2033,8 @@
           <t>ORD-10012</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2025-09-15</t>
-        </is>
+      <c r="B14" s="2" t="n">
+        <v>45915</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1580,24 +2063,20 @@
       <c r="I14" t="n">
         <v>1312561.7</v>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>2025-09-21 16:15</t>
-        </is>
+      <c r="J14" s="2" t="n">
+        <v>45921.67708333334</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>2025-09-16 16:15</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>2025-09-19 16:15</t>
-        </is>
+      <c r="L14" s="2" t="n">
+        <v>45919.67708333334</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1629,6 +2108,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>97µ</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>1048mm</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>CUST-A20LHW</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>555619578532</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>https://example.com/track/555619578532</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB14" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="15">
@@ -1637,14 +2159,12 @@
           <t>ORD-10013</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2025-06-18</t>
-        </is>
+      <c r="B15" s="2" t="n">
+        <v>45826</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>Film Extrusion</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1669,16 +2189,14 @@
       <c r="I15" t="n">
         <v>842444.8</v>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>2025-06-29 16:15</t>
-        </is>
+      <c r="J15" s="2" t="n">
+        <v>45887</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2025-08-17</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1710,6 +2228,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>76µ</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>532mm</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>CUST-WJO6TG</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB15" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="16">
@@ -1718,14 +2275,12 @@
           <t>ORD-10014</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2025-09-12</t>
-        </is>
+      <c r="B16" s="2" t="n">
+        <v>45912</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>Film Extrusion</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1750,16 +2305,14 @@
       <c r="I16" t="n">
         <v>1398297.6</v>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>2025-09-23 16:15</t>
-        </is>
+      <c r="J16" s="2" t="n">
+        <v>45973</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1791,6 +2344,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>85µ</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>1037mm</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>CUST-7XHO2V</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB16" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="17">
@@ -1799,14 +2391,12 @@
           <t>ORD-10015</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2025-11-20</t>
-        </is>
+      <c r="B17" s="2" t="n">
+        <v>45981</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1831,10 +2421,8 @@
       <c r="I17" t="n">
         <v>1090800</v>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>2025-11-24 16:15</t>
-        </is>
+      <c r="J17" s="2" t="n">
+        <v>46042</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1844,7 +2432,7 @@
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-03-06</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1876,6 +2464,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>105µ</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>578mm</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>CUST-Q94N0S</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>DTDC</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>732878771010</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>https://example.com/track/732878771010</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>In Transit</t>
+        </is>
+      </c>
+      <c r="AB17" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="18">
@@ -1884,14 +2515,12 @@
           <t>ORD-10016</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2025-08-21</t>
-        </is>
+      <c r="B18" s="2" t="n">
+        <v>45890</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>PO Received</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1916,16 +2545,14 @@
       <c r="I18" t="n">
         <v>7728</v>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>2025-08-25 16:15</t>
-        </is>
+      <c r="J18" s="2" t="n">
+        <v>45951</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1957,6 +2584,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>103µ</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>524mm</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>CUST-B86JGI</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB18" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -1965,10 +2631,8 @@
           <t>ORD-10017</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2025-11-02</t>
-        </is>
+      <c r="B19" s="2" t="n">
+        <v>45963</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1997,24 +2661,20 @@
       <c r="I19" t="n">
         <v>1152273.6</v>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>2025-11-07 16:15</t>
-        </is>
+      <c r="J19" s="2" t="n">
+        <v>45968.67708333334</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>2025-11-03 16:15</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>2025-11-05 16:15</t>
-        </is>
+      <c r="L19" s="2" t="n">
+        <v>45966.67708333334</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2046,6 +2706,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>69µ</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>1115mm</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>CUST-T5YNRA</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Blue Dart</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>274260041067</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>https://example.com/track/274260041067</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB19" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -2054,14 +2757,12 @@
           <t>ORD-10018</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2025-06-18</t>
-        </is>
+      <c r="B20" s="2" t="n">
+        <v>45826</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>QC</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2086,16 +2787,14 @@
       <c r="I20" t="n">
         <v>1063805.6</v>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>2025-06-26 16:15</t>
-        </is>
+      <c r="J20" s="2" t="n">
+        <v>45887</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2025-08-17</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -2127,6 +2826,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>82µ</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>619mm</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>CUST-3VLJIY</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB20" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="21">
@@ -2135,14 +2873,12 @@
           <t>ORD-10019</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2025-05-27</t>
-        </is>
+      <c r="B21" s="2" t="n">
+        <v>45804</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>PO Received</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2167,16 +2903,14 @@
       <c r="I21" t="n">
         <v>91728</v>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>2025-05-31 16:15</t>
-        </is>
+      <c r="J21" s="2" t="n">
+        <v>45865</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2025-07-26</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2208,6 +2942,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>42µ</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>483mm</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>CUST-EVET6I</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB21" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -2216,14 +2989,12 @@
           <t>ORD-10020</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2025-11-04</t>
-        </is>
+      <c r="B22" s="2" t="n">
+        <v>45965</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>QC</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2248,16 +3019,14 @@
       <c r="I22" t="n">
         <v>392882</v>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>2025-11-12 16:15</t>
-        </is>
+      <c r="J22" s="2" t="n">
+        <v>46026</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2289,6 +3058,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>119µ</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>621mm</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>CUST-Q772ZX</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB22" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="23">
@@ -2297,10 +3105,8 @@
           <t>ORD-10021</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2025-07-23</t>
-        </is>
+      <c r="B23" s="2" t="n">
+        <v>45861</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -2329,24 +3135,20 @@
       <c r="I23" t="n">
         <v>1015907.2</v>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>2025-08-01 16:15</t>
-        </is>
+      <c r="J23" s="2" t="n">
+        <v>45870.67708333334</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
           <t>2025-07-25 16:15</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>2025-07-28 16:15</t>
-        </is>
+      <c r="L23" s="2" t="n">
+        <v>45866.67708333334</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2025-09-21</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2378,6 +3180,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>105µ</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>645mm</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>CUST-T59JHA</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>Delhivery</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>317409084210</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>https://example.com/track/317409084210</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB23" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="24">
@@ -2386,14 +3231,12 @@
           <t>ORD-10022</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2025-10-22</t>
-        </is>
+      <c r="B24" s="2" t="n">
+        <v>45952</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2418,10 +3261,8 @@
       <c r="I24" t="n">
         <v>1404540</v>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>2025-10-24 16:15</t>
-        </is>
+      <c r="J24" s="2" t="n">
+        <v>46013</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2431,7 +3272,7 @@
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2026-03-22</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2463,6 +3304,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>40µ</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>695mm</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>CUST-DDU1MB</t>
+        </is>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>FedEx</t>
+        </is>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>443847037654</t>
+        </is>
+      </c>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>https://example.com/track/443847037654</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>Out for Delivery</t>
+        </is>
+      </c>
+      <c r="AB24" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="25">
@@ -2471,10 +3355,8 @@
           <t>ORD-10023</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>2025-09-19</t>
-        </is>
+      <c r="B25" s="2" t="n">
+        <v>45919</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -2503,24 +3385,20 @@
       <c r="I25" t="n">
         <v>495720</v>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>2025-09-24 16:15</t>
-        </is>
+      <c r="J25" s="2" t="n">
+        <v>45924.67708333334</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
           <t>2025-09-22 16:15</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>2025-09-26 16:15</t>
-        </is>
+      <c r="L25" s="2" t="n">
+        <v>45926.67708333334</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2552,6 +3430,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>117µ</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>625mm</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>CUST-QFKY7L</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>931428136428</t>
+        </is>
+      </c>
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>https://example.com/track/931428136428</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB25" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="26">
@@ -2560,14 +3481,12 @@
           <t>ORD-10024</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>2025-06-23</t>
-        </is>
+      <c r="B26" s="2" t="n">
+        <v>45831</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Printing</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2592,16 +3511,14 @@
       <c r="I26" t="n">
         <v>2047248</v>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>2025-07-05 16:15</t>
-        </is>
+      <c r="J26" s="2" t="n">
+        <v>45892</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2633,6 +3550,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>115µ</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>387mm</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>CUST-7436VT</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB26" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="27">
@@ -2641,10 +3597,8 @@
           <t>ORD-10025</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2025-08-04</t>
-        </is>
+      <c r="B27" s="2" t="n">
+        <v>45873</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -2673,24 +3627,20 @@
       <c r="I27" t="n">
         <v>2120398</v>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>2025-08-07 16:15</t>
-        </is>
+      <c r="J27" s="2" t="n">
+        <v>45876.67708333334</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
           <t>2025-08-05 16:15</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>2025-08-08 16:15</t>
-        </is>
+      <c r="L27" s="2" t="n">
+        <v>45877.67708333334</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2722,6 +3672,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>94µ</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>1021mm</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>CUST-2EID6E</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>708660613340</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>https://example.com/track/708660613340</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB27" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="28">
@@ -2730,14 +3723,12 @@
           <t>ORD-10026</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>2025-09-13</t>
-        </is>
+      <c r="B28" s="2" t="n">
+        <v>45913</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>PO Received</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2762,16 +3753,14 @@
       <c r="I28" t="n">
         <v>1130976</v>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>2025-09-21 16:15</t>
-        </is>
+      <c r="J28" s="2" t="n">
+        <v>45974</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -2803,6 +3792,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>43µ</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>594mm</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>CUST-J1U6QX</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB28" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="29">
@@ -2811,14 +3839,12 @@
           <t>ORD-10027</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2025-10-10</t>
-        </is>
+      <c r="B29" s="2" t="n">
+        <v>45940</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2843,10 +3869,8 @@
       <c r="I29" t="n">
         <v>644598</v>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>2025-10-15 16:15</t>
-        </is>
+      <c r="J29" s="2" t="n">
+        <v>46001</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -2856,7 +3880,7 @@
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2026-03-10</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -2888,6 +3912,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>91µ</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>311mm</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>CUST-YLBEIL</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>Blue Dart</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>130298875825</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>https://example.com/track/130298875825</t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>In Transit</t>
+        </is>
+      </c>
+      <c r="AB29" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="30">
@@ -2896,14 +3963,12 @@
           <t>ORD-10028</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2025-08-08</t>
-        </is>
+      <c r="B30" s="2" t="n">
+        <v>45877</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2928,10 +3993,8 @@
       <c r="I30" t="n">
         <v>212040</v>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>2025-08-15 16:15</t>
-        </is>
+      <c r="J30" s="2" t="n">
+        <v>45938</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -2941,7 +4004,7 @@
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -2973,6 +4036,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>108µ</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>670mm</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>CUST-RZO4Y4</t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>FedEx</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>657185265912</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>https://example.com/track/657185265912</t>
+        </is>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>Out for Delivery</t>
+        </is>
+      </c>
+      <c r="AB30" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="31">
@@ -2981,14 +4087,12 @@
           <t>ORD-10029</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>2025-09-17</t>
-        </is>
+      <c r="B31" s="2" t="n">
+        <v>45917</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Lamination</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3013,16 +4117,14 @@
       <c r="I31" t="n">
         <v>590127.2</v>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>2025-09-21 16:15</t>
-        </is>
+      <c r="J31" s="2" t="n">
+        <v>45978</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr">
         <is>
-          <t>2025-11-16</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -3054,6 +4156,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>72µ</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>366mm</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>CUST-MF5DHE</t>
+        </is>
+      </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB31" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="32">
@@ -3062,14 +4203,12 @@
           <t>ORD-10030</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>2025-09-23</t>
-        </is>
+      <c r="B32" s="2" t="n">
+        <v>45923</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Lamination</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3094,16 +4233,14 @@
       <c r="I32" t="n">
         <v>594092.8</v>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>2025-10-01 16:15</t>
-        </is>
+      <c r="J32" s="2" t="n">
+        <v>45984</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2026-02-21</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3135,6 +4272,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>81µ</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>1062mm</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>CUST-HT7XJ1</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB32" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="33">
@@ -3143,14 +4319,12 @@
           <t>ORD-10031</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>2025-08-04</t>
-        </is>
+      <c r="B33" s="2" t="n">
+        <v>45873</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -3175,10 +4349,8 @@
       <c r="I33" t="n">
         <v>179338.9</v>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>2025-08-07 16:15</t>
-        </is>
+      <c r="J33" s="2" t="n">
+        <v>45934</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
@@ -3188,7 +4360,7 @@
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -3220,6 +4392,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>80µ</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>924mm</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>CUST-G2TAY8</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>613545242477</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t>https://example.com/track/613545242477</t>
+        </is>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t>Out for Delivery</t>
+        </is>
+      </c>
+      <c r="AB33" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="34">
@@ -3228,14 +4443,12 @@
           <t>ORD-10032</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>2025-09-25</t>
-        </is>
+      <c r="B34" s="2" t="n">
+        <v>45925</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>PO Received</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -3260,16 +4473,14 @@
       <c r="I34" t="n">
         <v>2488903.2</v>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>2025-10-06 16:15</t>
-        </is>
+      <c r="J34" s="2" t="n">
+        <v>45986</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -3301,6 +4512,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>55µ</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>925mm</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>CUST-CPBJ49</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB34" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="35">
@@ -3309,14 +4559,12 @@
           <t>ORD-10033</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>2025-10-01</t>
-        </is>
+      <c r="B35" s="2" t="n">
+        <v>45931</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>QC</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3341,16 +4589,14 @@
       <c r="I35" t="n">
         <v>1082350.2</v>
       </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>2025-10-07 16:15</t>
-        </is>
+      <c r="J35" s="2" t="n">
+        <v>45992</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -3382,6 +4628,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>104µ</t>
+        </is>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>1156mm</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>CUST-BCLWH7</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB35" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="36">
@@ -3390,14 +4675,12 @@
           <t>ORD-10034</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>2025-08-05</t>
-        </is>
+      <c r="B36" s="2" t="n">
+        <v>45874</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>PO Received</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3422,16 +4705,14 @@
       <c r="I36" t="n">
         <v>763392</v>
       </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>2025-08-18 16:15</t>
-        </is>
+      <c r="J36" s="2" t="n">
+        <v>45935</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -3463,6 +4744,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>91µ</t>
+        </is>
+      </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>897mm</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>CUST-5IYZSU</t>
+        </is>
+      </c>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z36" t="inlineStr"/>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB36" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="37">
@@ -3471,10 +4791,8 @@
           <t>ORD-10035</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>2025-09-03</t>
-        </is>
+      <c r="B37" s="2" t="n">
+        <v>45903</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -3503,24 +4821,20 @@
       <c r="I37" t="n">
         <v>2255218.2</v>
       </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>2025-09-13 16:15</t>
-        </is>
+      <c r="J37" s="2" t="n">
+        <v>45913.67708333334</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
           <t>2025-09-06 16:15</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>2025-09-09 16:15</t>
-        </is>
+      <c r="L37" s="2" t="n">
+        <v>45909.67708333334</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>2025-11-02</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -3552,6 +4866,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>55µ</t>
+        </is>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>355mm</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>CUST-S9BNP5</t>
+        </is>
+      </c>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>FedEx</t>
+        </is>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>112965774354</t>
+        </is>
+      </c>
+      <c r="Z37" t="inlineStr">
+        <is>
+          <t>https://example.com/track/112965774354</t>
+        </is>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB37" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="38">
@@ -3560,14 +4917,12 @@
           <t>ORD-10036</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>2025-07-28</t>
-        </is>
+      <c r="B38" s="2" t="n">
+        <v>45866</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3592,10 +4947,8 @@
       <c r="I38" t="n">
         <v>1470150</v>
       </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>2025-07-31 16:15</t>
-        </is>
+      <c r="J38" s="2" t="n">
+        <v>45928</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -3605,7 +4958,7 @@
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -3637,6 +4990,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>108µ</t>
+        </is>
+      </c>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>392mm</t>
+        </is>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>CUST-Y9O8F8</t>
+        </is>
+      </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>FedEx</t>
+        </is>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>279660771829</t>
+        </is>
+      </c>
+      <c r="Z38" t="inlineStr">
+        <is>
+          <t>https://example.com/track/279660771829</t>
+        </is>
+      </c>
+      <c r="AA38" t="inlineStr">
+        <is>
+          <t>Out for Delivery</t>
+        </is>
+      </c>
+      <c r="AB38" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="39">
@@ -3645,14 +5041,12 @@
           <t>ORD-10037</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
+      <c r="B39" s="2" t="n">
+        <v>45869</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3677,10 +5071,8 @@
       <c r="I39" t="n">
         <v>292911.6</v>
       </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>2025-08-05 16:15</t>
-        </is>
+      <c r="J39" s="2" t="n">
+        <v>45930</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -3690,7 +5082,7 @@
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
@@ -3722,6 +5114,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>64µ</t>
+        </is>
+      </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>846mm</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>CUST-OPP45Q</t>
+        </is>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>DTDC</t>
+        </is>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>992858192209</t>
+        </is>
+      </c>
+      <c r="Z39" t="inlineStr">
+        <is>
+          <t>https://example.com/track/992858192209</t>
+        </is>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>Out for Delivery</t>
+        </is>
+      </c>
+      <c r="AB39" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="40">
@@ -3730,14 +5165,12 @@
           <t>ORD-10038</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2025-07-25</t>
-        </is>
+      <c r="B40" s="2" t="n">
+        <v>45863</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>Lamination</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3762,16 +5195,14 @@
       <c r="I40" t="n">
         <v>2277960</v>
       </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>2025-08-02 16:15</t>
-        </is>
+      <c r="J40" s="2" t="n">
+        <v>45925</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -3803,6 +5234,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>44µ</t>
+        </is>
+      </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>770mm</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>CUST-9SWING</t>
+        </is>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z40" t="inlineStr"/>
+      <c r="AA40" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB40" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="41">
@@ -3811,14 +5281,12 @@
           <t>ORD-10039</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>2025-09-04</t>
-        </is>
+      <c r="B41" s="2" t="n">
+        <v>45904</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Film Extrusion</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3843,16 +5311,14 @@
       <c r="I41" t="n">
         <v>2174512.8</v>
       </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>2025-09-13 16:15</t>
-        </is>
+      <c r="J41" s="2" t="n">
+        <v>45965</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -3884,6 +5350,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>PET / ALU / PE</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>115µ</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>697mm</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>CUST-DSL7RU</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z41" t="inlineStr"/>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB41" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="42">
@@ -3892,14 +5397,12 @@
           <t>ORD-10040</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>2025-07-18</t>
-        </is>
+      <c r="B42" s="2" t="n">
+        <v>45856</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3924,10 +5427,8 @@
       <c r="I42" t="n">
         <v>2610000</v>
       </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>2025-07-26 16:15</t>
-        </is>
+      <c r="J42" s="2" t="n">
+        <v>45918</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -3937,7 +5438,7 @@
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
@@ -3969,6 +5470,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>94µ</t>
+        </is>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>422mm</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>CUST-OR0NTY</t>
+        </is>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>DTDC</t>
+        </is>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>782062524151</t>
+        </is>
+      </c>
+      <c r="Z42" t="inlineStr">
+        <is>
+          <t>https://example.com/track/782062524151</t>
+        </is>
+      </c>
+      <c r="AA42" t="inlineStr">
+        <is>
+          <t>In Transit</t>
+        </is>
+      </c>
+      <c r="AB42" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="43">
@@ -3977,14 +5521,12 @@
           <t>ORD-10041</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>2025-10-15</t>
-        </is>
+      <c r="B43" s="2" t="n">
+        <v>45945</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -4009,10 +5551,8 @@
       <c r="I43" t="n">
         <v>2314656</v>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>2025-10-19 16:15</t>
-        </is>
+      <c r="J43" s="2" t="n">
+        <v>46006</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -4022,7 +5562,7 @@
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -4054,6 +5594,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>83µ</t>
+        </is>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>597mm</t>
+        </is>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>CUST-G4J9BB</t>
+        </is>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>Delhivery</t>
+        </is>
+      </c>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>685160229587</t>
+        </is>
+      </c>
+      <c r="Z43" t="inlineStr">
+        <is>
+          <t>https://example.com/track/685160229587</t>
+        </is>
+      </c>
+      <c r="AA43" t="inlineStr">
+        <is>
+          <t>Out for Delivery</t>
+        </is>
+      </c>
+      <c r="AB43" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="44">
@@ -4062,14 +5645,12 @@
           <t>ORD-10042</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>2025-08-04</t>
-        </is>
+      <c r="B44" s="2" t="n">
+        <v>45873</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ordered</t>
+          <t>Film Extrusion</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -4094,16 +5675,14 @@
       <c r="I44" t="n">
         <v>1408322.5</v>
       </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>2025-08-16 16:15</t>
-        </is>
+      <c r="J44" s="2" t="n">
+        <v>45934</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -4135,6 +5714,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>82µ</t>
+        </is>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>1042mm</t>
+        </is>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>CUST-MWJ1VI</t>
+        </is>
+      </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z44" t="inlineStr"/>
+      <c r="AA44" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB44" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="45">
@@ -4143,14 +5761,12 @@
           <t>ORD-10043</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>2025-08-06</t>
-        </is>
+      <c r="B45" s="2" t="n">
+        <v>45875</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>PO Received</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -4175,16 +5791,14 @@
       <c r="I45" t="n">
         <v>1399794</v>
       </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>2025-08-14 16:15</t>
-        </is>
+      <c r="J45" s="2" t="n">
+        <v>45936</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr">
         <is>
-          <t>2025-10-05</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -4216,6 +5830,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>87µ</t>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>960mm</t>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>CUST-X00AVN</t>
+        </is>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z45" t="inlineStr"/>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB45" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="46">
@@ -4224,10 +5877,8 @@
           <t>ORD-10044</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>2025-07-28</t>
-        </is>
+      <c r="B46" s="2" t="n">
+        <v>45866</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -4256,24 +5907,20 @@
       <c r="I46" t="n">
         <v>590579.2</v>
       </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>2025-08-05 16:15</t>
-        </is>
+      <c r="J46" s="2" t="n">
+        <v>45874.67708333334</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
           <t>2025-07-31 16:15</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>2025-08-04 16:15</t>
-        </is>
+      <c r="L46" s="2" t="n">
+        <v>45873.67708333334</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -4305,6 +5952,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>48µ</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>1032mm</t>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>CUST-T0418V</t>
+        </is>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>FedEx</t>
+        </is>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>945147451725</t>
+        </is>
+      </c>
+      <c r="Z46" t="inlineStr">
+        <is>
+          <t>https://example.com/track/945147451725</t>
+        </is>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB46" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="47">
@@ -4313,14 +6003,12 @@
           <t>ORD-10045</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>2025-11-14</t>
-        </is>
+      <c r="B47" s="2" t="n">
+        <v>45975</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Printing</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -4345,16 +6033,14 @@
       <c r="I47" t="n">
         <v>564710.4</v>
       </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>2025-11-23 16:15</t>
-        </is>
+      <c r="J47" s="2" t="n">
+        <v>46036</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-02-28</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -4386,6 +6072,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>74µ</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>925mm</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>CUST-1V9EXU</t>
+        </is>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z47" t="inlineStr"/>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB47" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="48">
@@ -4394,14 +6119,12 @@
           <t>ORD-10046</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>2025-08-10</t>
-        </is>
+      <c r="B48" s="2" t="n">
+        <v>45879</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Shipped</t>
+          <t>Dispatch</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4426,10 +6149,8 @@
       <c r="I48" t="n">
         <v>250458</v>
       </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>2025-08-18 16:15</t>
-        </is>
+      <c r="J48" s="2" t="n">
+        <v>45940</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -4439,7 +6160,7 @@
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
@@ -4471,6 +6192,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>PET 12µ / PE 50µ</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>65µ</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>583mm</t>
+        </is>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>CUST-W2EZK1</t>
+        </is>
+      </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>Delhivery</t>
+        </is>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>648956485660</t>
+        </is>
+      </c>
+      <c r="Z48" t="inlineStr">
+        <is>
+          <t>https://example.com/track/648956485660</t>
+        </is>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t>Out for Delivery</t>
+        </is>
+      </c>
+      <c r="AB48" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="49">
@@ -4479,14 +6243,12 @@
           <t>ORD-10047</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>2025-09-03</t>
-        </is>
+      <c r="B49" s="2" t="n">
+        <v>45903</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Lamination</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4511,16 +6273,14 @@
       <c r="I49" t="n">
         <v>439482</v>
       </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>2025-09-13 16:15</t>
-        </is>
+      <c r="J49" s="2" t="n">
+        <v>45964</v>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr">
         <is>
-          <t>2025-11-02</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
@@ -4552,6 +6312,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>PET / PE / EVOH / PE</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>49µ</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>707mm</t>
+        </is>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>CUST-7BMTLN</t>
+        </is>
+      </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z49" t="inlineStr"/>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB49" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="50">
@@ -4560,14 +6359,12 @@
           <t>ORD-10048</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>2025-08-16</t>
-        </is>
+      <c r="B50" s="2" t="n">
+        <v>45885</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>QC</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4592,16 +6389,14 @@
       <c r="I50" t="n">
         <v>1001560</v>
       </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>2025-08-25 16:15</t>
-        </is>
+      <c r="J50" s="2" t="n">
+        <v>45946</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -4633,6 +6428,45 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>BOPP / MET PET / PE</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>105µ</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>634mm</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>CUST-FP1WOJ</t>
+        </is>
+      </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="Z50" t="inlineStr"/>
+      <c r="AA50" t="inlineStr">
+        <is>
+          <t>Pending Dispatch</t>
+        </is>
+      </c>
+      <c r="AB50" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="51">
@@ -4641,10 +6475,8 @@
           <t>ORD-10049</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>2025-11-14</t>
-        </is>
+      <c r="B51" s="2" t="n">
+        <v>45975</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -4673,24 +6505,20 @@
       <c r="I51" t="n">
         <v>1014208</v>
       </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>2025-11-21 16:15</t>
-        </is>
+      <c r="J51" s="2" t="n">
+        <v>45982.67708333334</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
           <t>2025-11-17 16:15</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>2025-11-20 16:15</t>
-        </is>
+      <c r="L51" s="2" t="n">
+        <v>45981.67708333334</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -4722,6 +6550,49 @@
         <is>
           <t>TIN5676780000</t>
         </is>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>BOPP 20µ / PE 40µ</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>83µ</t>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>896mm</t>
+        </is>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>CUST-1BTCN7</t>
+        </is>
+      </c>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>792895264363</t>
+        </is>
+      </c>
+      <c r="Z51" t="inlineStr">
+        <is>
+          <t>https://example.com/track/792895264363</t>
+        </is>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="AB51" t="n">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>